<commit_message>
Update custom shiny input function, upload new data dictionary
</commit_message>
<xml_diff>
--- a/app/files/template.xlsx
+++ b/app/files/template.xlsx
@@ -1,27 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyashapiro/Desktop/soil-app-v2/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyashapiro/Desktop/Clients/wsda/soil-health-report-generator/app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B606110-9DB0-8A47-ACE6-F87D8AACAFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79157FA-8252-6D45-939F-6D1B82E25DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="760" windowWidth="13400" windowHeight="13420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="760" windowWidth="22760" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Data Dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="410">
   <si>
     <t>year</t>
   </si>
@@ -1106,265 +1119,151 @@
     <t>22-LJP05-03</t>
   </si>
   <si>
-    <t>measurement_group</t>
+    <t>column_name</t>
+  </si>
+  <si>
+    <t>abbr</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>Biological</t>
+  </si>
+  <si>
+    <t>Organic Matter</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Min C</t>
+  </si>
+  <si>
+    <t>mg/kg/day</t>
+  </si>
+  <si>
+    <t>POXC</t>
+  </si>
+  <si>
+    <t>ppm</t>
+  </si>
+  <si>
+    <t>PMN</t>
+  </si>
+  <si>
+    <t>lb/ac</t>
+  </si>
+  <si>
+    <t>ACE Protein</t>
+  </si>
+  <si>
+    <t>g/kg</t>
+  </si>
+  <si>
+    <t>Chemical</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>mmhos/cm</t>
+  </si>
+  <si>
+    <t>CEC</t>
+  </si>
+  <si>
+    <t>cmolc/kg</t>
+  </si>
+  <si>
+    <t>Total C</t>
+  </si>
+  <si>
+    <t>TOC</t>
+  </si>
+  <si>
+    <t>Inorganic C</t>
+  </si>
+  <si>
+    <t>Plant Essential Macro Nutrients</t>
+  </si>
+  <si>
+    <t>Total N</t>
+  </si>
+  <si>
+    <t>NO₃-N</t>
+  </si>
+  <si>
+    <t>NH₄-N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Ca</t>
+  </si>
+  <si>
+    <t>Mg</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Plant Essential Micro Nutrients</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Fe</t>
+  </si>
+  <si>
+    <t>Mn</t>
+  </si>
+  <si>
+    <t>Cu</t>
+  </si>
+  <si>
+    <t>Zn</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Sand</t>
+  </si>
+  <si>
+    <t>Silt</t>
+  </si>
+  <si>
+    <t>Bulk Density</t>
+  </si>
+  <si>
+    <t>g/cm³</t>
+  </si>
+  <si>
+    <t>Agg. Stability</t>
+  </si>
+  <si>
+    <t>WHC</t>
+  </si>
+  <si>
+    <t>in/ft</t>
+  </si>
+  <si>
+    <t>Texture</t>
   </si>
   <si>
     <t>measurement_group_label</t>
-  </si>
-  <si>
-    <t>column_name</t>
-  </si>
-  <si>
-    <t>order</t>
-  </si>
-  <si>
-    <t>abbr</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>abbr_unit</t>
-  </si>
-  <si>
-    <t>biological</t>
-  </si>
-  <si>
-    <t>Biological</t>
-  </si>
-  <si>
-    <t>Organic Matter</t>
-  </si>
-  <si>
-    <t>%</t>
-  </si>
-  <si>
-    <t>Organic Matter&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>Min C</t>
-  </si>
-  <si>
-    <t>mg/kg/day</t>
-  </si>
-  <si>
-    <t>Min C&lt;br&gt;(mg/kg/day)</t>
-  </si>
-  <si>
-    <t>POXC</t>
-  </si>
-  <si>
-    <t>ppm</t>
-  </si>
-  <si>
-    <t>POXC&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>PMN</t>
-  </si>
-  <si>
-    <t>lb/ac</t>
-  </si>
-  <si>
-    <t>PMN&lt;br&gt;(lb/ac)</t>
-  </si>
-  <si>
-    <t>ACE Protein</t>
-  </si>
-  <si>
-    <t>g/kg</t>
-  </si>
-  <si>
-    <t>ACE Protein&lt;br&gt;(g/kg)</t>
-  </si>
-  <si>
-    <t>chemical</t>
-  </si>
-  <si>
-    <t>Chemical</t>
-  </si>
-  <si>
-    <t>pH</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>EC</t>
-  </si>
-  <si>
-    <t>mmhos/cm</t>
-  </si>
-  <si>
-    <t>EC&lt;br&gt;(mmhos/cm)</t>
-  </si>
-  <si>
-    <t>CEC</t>
-  </si>
-  <si>
-    <t>cmolc/kg</t>
-  </si>
-  <si>
-    <t>CEC&lt;br&gt;(cmolc/kg)</t>
-  </si>
-  <si>
-    <t>Total C</t>
-  </si>
-  <si>
-    <t>Total C&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>TOC</t>
-  </si>
-  <si>
-    <t>TOC&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>Inorganic C</t>
-  </si>
-  <si>
-    <t>Inorganic C&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>macro</t>
-  </si>
-  <si>
-    <t>Plant Essential Macro Nutrients</t>
-  </si>
-  <si>
-    <t>Total N</t>
-  </si>
-  <si>
-    <t>Total N&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>NO₃-N</t>
-  </si>
-  <si>
-    <t>NO₃-N&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>NH₄-N</t>
-  </si>
-  <si>
-    <t>NH₄-N&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>P&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>K&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Ca</t>
-  </si>
-  <si>
-    <t>Ca&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Mg</t>
-  </si>
-  <si>
-    <t>Mg&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>S&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>micro</t>
-  </si>
-  <si>
-    <t>Plant Essential Micro Nutrients</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>B&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Fe</t>
-  </si>
-  <si>
-    <t>Fe&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Mn</t>
-  </si>
-  <si>
-    <t>Mn&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Cu</t>
-  </si>
-  <si>
-    <t>Cu&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Zn</t>
-  </si>
-  <si>
-    <t>Zn&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>Na</t>
-  </si>
-  <si>
-    <t>Na&lt;br&gt;(ppm)</t>
-  </si>
-  <si>
-    <t>physical</t>
-  </si>
-  <si>
-    <t>Physical</t>
-  </si>
-  <si>
-    <t>Sand</t>
-  </si>
-  <si>
-    <t>Sand&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>Silt</t>
-  </si>
-  <si>
-    <t>Silt&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>Clay&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>Bulk Density</t>
-  </si>
-  <si>
-    <t>g/cm³</t>
-  </si>
-  <si>
-    <t>Bulk Density&lt;br&gt;(g/cm³)</t>
-  </si>
-  <si>
-    <t>Agg. Stability</t>
-  </si>
-  <si>
-    <t>Agg. Stability&lt;br&gt;(%)</t>
-  </si>
-  <si>
-    <t>WHC</t>
-  </si>
-  <si>
-    <t>in/ft</t>
-  </si>
-  <si>
-    <t>WHC&lt;br&gt;(in/ft)</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AP101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -14370,748 +14271,474 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>409</v>
+      </c>
+      <c r="B1" t="s">
         <v>361</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>362</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>363</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>401</v>
+      </c>
+      <c r="D3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>402</v>
+      </c>
+      <c r="D4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>400</v>
+      </c>
+      <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>400</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>403</v>
+      </c>
+      <c r="D6" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>400</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>405</v>
+      </c>
+      <c r="D7" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>406</v>
+      </c>
+      <c r="D8" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>364</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
         <v>365</v>
       </c>
-      <c r="F1" t="s">
+      <c r="D9" t="s">
         <v>366</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>364</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
         <v>367</v>
       </c>
+      <c r="D10" t="s">
+        <v>368</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
         <v>369</v>
       </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D11" t="s">
         <v>370</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>364</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
         <v>371</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D12" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>368</v>
-      </c>
-      <c r="B3" t="s">
-        <v>369</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
         <v>373</v>
       </c>
-      <c r="F3" t="s">
+      <c r="D13" t="s">
         <v>374</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>375</v>
       </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>376</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>368</v>
-      </c>
-      <c r="B4" t="s">
-        <v>369</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>376</v>
-      </c>
-      <c r="F4" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>375</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
         <v>377</v>
       </c>
-      <c r="G4" t="s">
+      <c r="D15" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>368</v>
-      </c>
-      <c r="B5" t="s">
-        <v>369</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>375</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
         <v>379</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D16" t="s">
         <v>380</v>
       </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>375</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
         <v>381</v>
       </c>
+      <c r="D17" t="s">
+        <v>366</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>368</v>
-      </c>
-      <c r="B6" t="s">
-        <v>369</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>375</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
         <v>382</v>
       </c>
-      <c r="F6" t="s">
+      <c r="D18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>375</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
         <v>383</v>
       </c>
-      <c r="G6" t="s">
+      <c r="D19" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>384</v>
       </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>385</v>
+      </c>
+      <c r="D20" t="s">
+        <v>366</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>385</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>384</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
         <v>386</v>
       </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="D21" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>384</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
         <v>387</v>
       </c>
-      <c r="F7" t="s">
+      <c r="D22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>384</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" t="s">
         <v>388</v>
       </c>
-      <c r="G7" t="s">
-        <v>387</v>
+      <c r="D23" t="s">
+        <v>370</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>385</v>
-      </c>
-      <c r="B8" t="s">
-        <v>386</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>384</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" t="s">
         <v>389</v>
       </c>
-      <c r="F8" t="s">
+      <c r="D24" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>384</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
         <v>390</v>
       </c>
-      <c r="G8" t="s">
+      <c r="D25" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>384</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
         <v>391</v>
       </c>
+      <c r="D26" t="s">
+        <v>370</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>385</v>
-      </c>
-      <c r="B9" t="s">
-        <v>386</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>384</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
         <v>392</v>
       </c>
-      <c r="F9" t="s">
+      <c r="D27" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>393</v>
       </c>
-      <c r="G9" t="s">
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="s">
         <v>394</v>
       </c>
+      <c r="D28" t="s">
+        <v>370</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>385</v>
-      </c>
-      <c r="B10" t="s">
-        <v>386</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>393</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
         <v>395</v>
       </c>
-      <c r="F10" t="s">
-        <v>371</v>
-      </c>
-      <c r="G10" t="s">
+      <c r="D29" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>393</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
         <v>396</v>
       </c>
+      <c r="D30" t="s">
+        <v>370</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>385</v>
-      </c>
-      <c r="B11" t="s">
-        <v>386</v>
-      </c>
-      <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="E11" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>393</v>
+      </c>
+      <c r="B31" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" t="s">
         <v>397</v>
       </c>
-      <c r="F11" t="s">
-        <v>371</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="D31" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>393</v>
+      </c>
+      <c r="B32" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" t="s">
         <v>398</v>
       </c>
+      <c r="D32" t="s">
+        <v>370</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>385</v>
-      </c>
-      <c r="B12" t="s">
-        <v>386</v>
-      </c>
-      <c r="C12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>393</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="s">
         <v>399</v>
       </c>
-      <c r="F12" t="s">
-        <v>371</v>
-      </c>
-      <c r="G12" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>401</v>
-      </c>
-      <c r="B13" t="s">
-        <v>402</v>
-      </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>403</v>
-      </c>
-      <c r="F13" t="s">
-        <v>371</v>
-      </c>
-      <c r="G13" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>401</v>
-      </c>
-      <c r="B14" t="s">
-        <v>402</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>405</v>
-      </c>
-      <c r="F14" t="s">
-        <v>377</v>
-      </c>
-      <c r="G14" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>401</v>
-      </c>
-      <c r="B15" t="s">
-        <v>402</v>
-      </c>
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>407</v>
-      </c>
-      <c r="F15" t="s">
-        <v>377</v>
-      </c>
-      <c r="G15" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>401</v>
-      </c>
-      <c r="B16" t="s">
-        <v>402</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>409</v>
-      </c>
-      <c r="F16" t="s">
-        <v>377</v>
-      </c>
-      <c r="G16" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>401</v>
-      </c>
-      <c r="B17" t="s">
-        <v>402</v>
-      </c>
-      <c r="C17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>411</v>
-      </c>
-      <c r="F17" t="s">
-        <v>377</v>
-      </c>
-      <c r="G17" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>401</v>
-      </c>
-      <c r="B18" t="s">
-        <v>402</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>413</v>
-      </c>
-      <c r="F18" t="s">
-        <v>377</v>
-      </c>
-      <c r="G18" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>401</v>
-      </c>
-      <c r="B19" t="s">
-        <v>402</v>
-      </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>415</v>
-      </c>
-      <c r="F19" t="s">
-        <v>377</v>
-      </c>
-      <c r="G19" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>401</v>
-      </c>
-      <c r="B20" t="s">
-        <v>402</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
-        <v>417</v>
-      </c>
-      <c r="F20" t="s">
-        <v>377</v>
-      </c>
-      <c r="G20" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>419</v>
-      </c>
-      <c r="B21" t="s">
-        <v>420</v>
-      </c>
-      <c r="C21" t="s">
-        <v>23</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>421</v>
-      </c>
-      <c r="F21" t="s">
-        <v>377</v>
-      </c>
-      <c r="G21" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>419</v>
-      </c>
-      <c r="B22" t="s">
-        <v>420</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D22">
-        <v>2</v>
-      </c>
-      <c r="E22" t="s">
-        <v>423</v>
-      </c>
-      <c r="F22" t="s">
-        <v>377</v>
-      </c>
-      <c r="G22" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>419</v>
-      </c>
-      <c r="B23" t="s">
-        <v>420</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>425</v>
-      </c>
-      <c r="F23" t="s">
-        <v>377</v>
-      </c>
-      <c r="G23" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>419</v>
-      </c>
-      <c r="B24" t="s">
-        <v>420</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24">
-        <v>4</v>
-      </c>
-      <c r="E24" t="s">
-        <v>427</v>
-      </c>
-      <c r="F24" t="s">
-        <v>377</v>
-      </c>
-      <c r="G24" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>419</v>
-      </c>
-      <c r="B25" t="s">
-        <v>420</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25">
-        <v>5</v>
-      </c>
-      <c r="E25" t="s">
-        <v>429</v>
-      </c>
-      <c r="F25" t="s">
-        <v>377</v>
-      </c>
-      <c r="G25" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>419</v>
-      </c>
-      <c r="B26" t="s">
-        <v>420</v>
-      </c>
-      <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>431</v>
-      </c>
-      <c r="F26" t="s">
-        <v>377</v>
-      </c>
-      <c r="G26" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>433</v>
-      </c>
-      <c r="B27" t="s">
-        <v>434</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>435</v>
-      </c>
-      <c r="F27" t="s">
-        <v>371</v>
-      </c>
-      <c r="G27" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>433</v>
-      </c>
-      <c r="B28" t="s">
-        <v>434</v>
-      </c>
-      <c r="C28" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28">
-        <v>2</v>
-      </c>
-      <c r="E28" t="s">
-        <v>437</v>
-      </c>
-      <c r="F28" t="s">
-        <v>371</v>
-      </c>
-      <c r="G28" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>433</v>
-      </c>
-      <c r="B29" t="s">
-        <v>434</v>
-      </c>
-      <c r="C29" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>161</v>
-      </c>
-      <c r="F29" t="s">
-        <v>371</v>
-      </c>
-      <c r="G29" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>433</v>
-      </c>
-      <c r="B30" t="s">
-        <v>434</v>
-      </c>
-      <c r="C30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <v>5</v>
-      </c>
-      <c r="E30" t="s">
-        <v>440</v>
-      </c>
-      <c r="F30" t="s">
-        <v>441</v>
-      </c>
-      <c r="G30" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>433</v>
-      </c>
-      <c r="B31" t="s">
-        <v>434</v>
-      </c>
-      <c r="C31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31">
-        <v>6</v>
-      </c>
-      <c r="E31" t="s">
-        <v>443</v>
-      </c>
-      <c r="F31" t="s">
-        <v>371</v>
-      </c>
-      <c r="G31" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>433</v>
-      </c>
-      <c r="B32" t="s">
-        <v>434</v>
-      </c>
-      <c r="C32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D32">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
-        <v>445</v>
-      </c>
-      <c r="F32" t="s">
-        <v>446</v>
-      </c>
-      <c r="G32" t="s">
-        <v>447</v>
+      <c r="D33" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update data validation function
</commit_message>
<xml_diff>
--- a/app/files/template.xlsx
+++ b/app/files/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanyashapiro/Desktop/Clients/wsda/soil-health-report-generator/app/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79157FA-8252-6D45-939F-6D1B82E25DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FBD170-90FA-CF48-997F-28A164A66C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="760" windowWidth="22760" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1263,7 +1263,7 @@
     <t>Texture</t>
   </si>
   <si>
-    <t>measurement_group_label</t>
+    <t>measurement_group</t>
   </si>
 </sst>
 </file>

</xml_diff>